<commit_message>
to run on chrome
</commit_message>
<xml_diff>
--- a/Urls_Int - Copy.xlsx
+++ b/Urls_Int - Copy.xlsx
@@ -19,34 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
-  <si>
-    <t>http://pp.avacon-netz.de/registrieren</t>
-  </si>
-  <si>
-    <t>http://pp.bayernwerk-netz.de/registrieren</t>
-  </si>
-  <si>
-    <t>http://pp.sh-netz.com/registrieren</t>
-  </si>
-  <si>
-    <t>http://pp.e-dis-netz.de/registrieren</t>
-  </si>
-  <si>
-    <t>http://pp.energienetze-schaafheim.com/registrieren</t>
-  </si>
-  <si>
-    <t>http://pp.hansegas.com/registrieren</t>
-  </si>
-  <si>
-    <t>http://pp.energienetze-bayern.com/registrieren</t>
-  </si>
-  <si>
-    <t>http://pp.gasnetz-hamburg.de/registrieren</t>
-  </si>
-  <si>
-    <t>http://pp.energieversorgung-putzbrunn.de/registrieren</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>http://int.avacon-netz.de/registrieren</t>
   </si>
@@ -72,46 +45,145 @@
     <t>http://int.energieversorgung-putzbrunn.de/registrieren</t>
   </si>
   <si>
-    <t>http://int.hh-netz.com/registrieren</t>
-  </si>
-  <si>
     <t>http://int.nordnetz.com/registrieren</t>
   </si>
   <si>
     <t>http://int.avacon-hochdrucknetz.de/registrieren</t>
   </si>
   <si>
-    <t>http://qa.avacon-netz.de/registrieren</t>
-  </si>
-  <si>
-    <t>http://qa.bayernwerk-netz.de/registrieren</t>
-  </si>
-  <si>
-    <t>http://qa.sh-netz.com/registrieren</t>
-  </si>
-  <si>
-    <t>http://qa.e-dis-netz.de/registrieren</t>
-  </si>
-  <si>
-    <t>http://qa.energienetze-schaafheim.com/registrieren</t>
-  </si>
-  <si>
-    <t>http://qa.hansegas.com/registrieren</t>
-  </si>
-  <si>
-    <t>http://qa.energienetze-bayern.com/registrieren</t>
-  </si>
-  <si>
-    <t>http://qa.energieversorgung-putzbrunn.de/registrieren</t>
-  </si>
-  <si>
-    <t>http://qa.nordnetz.com/registrieren</t>
-  </si>
-  <si>
-    <t>http://qa.avacon-hochdrucknetz.de/registrieren</t>
-  </si>
-  <si>
-    <t>http://qa.gasnetz-hamburg.de/registrieren</t>
+    <t>http://int.avacon-netz.de/passwort-vergessen</t>
+  </si>
+  <si>
+    <t>http://int.bayernwerk-netz.de/passwort-vergessen</t>
+  </si>
+  <si>
+    <t>http://int.sh-netz.com/passwort-vergessen</t>
+  </si>
+  <si>
+    <t>http://int.e-dis-netz.de/passwort-vergessen</t>
+  </si>
+  <si>
+    <t>http://int.energienetze-schaafheim.com/passwort-vergessen</t>
+  </si>
+  <si>
+    <t>http://int.hansegas.com/passwort-vergessen</t>
+  </si>
+  <si>
+    <t>http://int.energienetze-bayern.com/passwort-vergessen</t>
+  </si>
+  <si>
+    <t>http://int.energieversorgung-putzbrunn.de/passwort-vergessen</t>
+  </si>
+  <si>
+    <t>http://int.nordnetz.com/passwort-vergessen</t>
+  </si>
+  <si>
+    <t>http://int.avacon-hochdrucknetz.de/passwort-vergessen</t>
+  </si>
+  <si>
+    <t>http://int.avacon-netz.de/gastzugang</t>
+  </si>
+  <si>
+    <t>http://int.bayernwerk-netz.de/gastzugang</t>
+  </si>
+  <si>
+    <t>http://int.sh-netz.com/gastzugang</t>
+  </si>
+  <si>
+    <t>http://int.e-dis-netz.de/gastzugang</t>
+  </si>
+  <si>
+    <t>http://int.energienetze-schaafheim.com/gastzugang</t>
+  </si>
+  <si>
+    <t>http://int.hansegas.com/gastzugang</t>
+  </si>
+  <si>
+    <t>http://int.energienetze-bayern.com/gastzugang</t>
+  </si>
+  <si>
+    <t>http://int.energieversorgung-putzbrunn.de/gastzugang</t>
+  </si>
+  <si>
+    <t>http://int.nordnetz.com/gastzugang</t>
+  </si>
+  <si>
+    <t>http://int.avacon-hochdrucknetz.de/gastzugang</t>
+  </si>
+  <si>
+    <t>http://int.avacon-netz.de/login</t>
+  </si>
+  <si>
+    <t>http://int.bayernwerk-netz.de/login</t>
+  </si>
+  <si>
+    <t>http://int.sh-netz.com/login</t>
+  </si>
+  <si>
+    <t>http://int.e-dis-netz.de/login</t>
+  </si>
+  <si>
+    <t>http://int.energienetze-schaafheim.com/login</t>
+  </si>
+  <si>
+    <t>http://int.hansegas.com/login</t>
+  </si>
+  <si>
+    <t>http://int.energienetze-bayern.com/login</t>
+  </si>
+  <si>
+    <t>http://int.energieversorgung-putzbrunn.de/login</t>
+  </si>
+  <si>
+    <t>http://int.nordnetz.com/login</t>
+  </si>
+  <si>
+    <t>http://int.avacon-hochdrucknetz.de/login</t>
+  </si>
+  <si>
+    <t>http://int.avacon-netz.de/kundenportal</t>
+  </si>
+  <si>
+    <t>http://int.bayernwerk-netz.de/kundenportal</t>
+  </si>
+  <si>
+    <t>http://int.sh-netz.com/kundenportal</t>
+  </si>
+  <si>
+    <t>http://int.e-dis-netz.de/kundenportal</t>
+  </si>
+  <si>
+    <t>http://int.energienetze-schaafheim.com/kundenportal</t>
+  </si>
+  <si>
+    <t>http://int.hansegas.com/kundenportal</t>
+  </si>
+  <si>
+    <t>http://int.energienetze-bayern.com/kundenportal</t>
+  </si>
+  <si>
+    <t>http://int.energieversorgung-putzbrunn.de/kundenportal</t>
+  </si>
+  <si>
+    <t>http://int.nordnetz.com/kundenportal</t>
+  </si>
+  <si>
+    <t>http://int.avacon-hochdrucknetz.de/kundenportal</t>
+  </si>
+  <si>
+    <t>http://int.gasnetz-hamburg.de/gastzugang</t>
+  </si>
+  <si>
+    <t>http://int.gasnetz-hamburg.de/login</t>
+  </si>
+  <si>
+    <t>http://int.gasnetz-hamburg.de/kundenportal</t>
+  </si>
+  <si>
+    <t>http://int.gasnetz-hamburg.de/registrieren</t>
+  </si>
+  <si>
+    <t>http://int.gasnetz-hamburg.de/passwort-vergessen</t>
   </si>
 </sst>
 </file>
@@ -429,15 +501,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A31"/>
+  <dimension ref="A1:A55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" customWidth="1"/>
+    <col min="1" max="1" width="61.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -477,52 +549,52 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -532,93 +604,196 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A10" r:id="rId1"/>
-    <hyperlink ref="A11" r:id="rId2"/>
-    <hyperlink ref="A12" r:id="rId3"/>
-    <hyperlink ref="A13" r:id="rId4"/>
-    <hyperlink ref="A14" r:id="rId5"/>
-    <hyperlink ref="A15" r:id="rId6"/>
-    <hyperlink ref="A16" r:id="rId7"/>
-    <hyperlink ref="A17" r:id="rId8"/>
-    <hyperlink ref="A18" r:id="rId9"/>
-    <hyperlink ref="A19" r:id="rId10"/>
-    <hyperlink ref="A20" r:id="rId11"/>
-    <hyperlink ref="A21" r:id="rId12"/>
-    <hyperlink ref="A22" r:id="rId13"/>
-    <hyperlink ref="A23" r:id="rId14"/>
-    <hyperlink ref="A24" r:id="rId15"/>
-    <hyperlink ref="A25" r:id="rId16"/>
-    <hyperlink ref="A26" r:id="rId17"/>
-    <hyperlink ref="A27" r:id="rId18"/>
-    <hyperlink ref="A28" r:id="rId19"/>
-    <hyperlink ref="A29" r:id="rId20"/>
-    <hyperlink ref="A30" r:id="rId21"/>
-    <hyperlink ref="A31" r:id="rId22"/>
+    <hyperlink ref="A8" r:id="rId1"/>
+    <hyperlink ref="A19" r:id="rId2"/>
+    <hyperlink ref="A30" r:id="rId3"/>
+    <hyperlink ref="A41" r:id="rId4"/>
+    <hyperlink ref="A52" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>